<commit_message>
new improvements in the code
</commit_message>
<xml_diff>
--- a/2 PART MIXTURE/Tables.xlsx
+++ b/2 PART MIXTURE/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\RAND_pro\prog_calc\prog_calc2\2 PART MIXTURE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE4E937F-2B19-4137-8860-80E0E2D9AE08}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1AA6F1-A492-416C-BB0E-5E5E97BC0020}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03F6D715-826B-4640-9764-84D30B4B9310}"/>
   </bookViews>
@@ -96,13 +96,13 @@
     <t>users</t>
   </si>
   <si>
-    <t xml:space="preserve">What is the problem? Tobit appears to be the best </t>
-  </si>
-  <si>
-    <t>model for low and high, we need to build a model that does</t>
-  </si>
-  <si>
-    <t>better on high</t>
+    <t xml:space="preserve">What is the problem? Tobit appears to be the 3d best </t>
+  </si>
+  <si>
+    <t xml:space="preserve">model for low and high, we need to build a model that shows that tobit </t>
+  </si>
+  <si>
+    <t>does not to good at high</t>
   </si>
 </sst>
 </file>
@@ -209,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -250,6 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65379297-C1EA-45C9-BB46-CC2BA0E9752C}">
-  <dimension ref="B5:AG39"/>
+  <dimension ref="B5:AG44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J19" workbookViewId="0">
-      <selection activeCell="AB37" sqref="AB37"/>
+    <sheetView tabSelected="1" topLeftCell="J22" workbookViewId="0">
+      <selection activeCell="Y39" sqref="Y39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1327,7 +1328,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="16:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="16:25" x14ac:dyDescent="0.3">
       <c r="P33" s="10" t="s">
         <v>0</v>
       </c>
@@ -1344,13 +1345,14 @@
         <v>291.1773</v>
       </c>
       <c r="V33" s="5">
-        <v>281.75063999999998</v>
+        <v>282.1859</v>
       </c>
       <c r="W33" s="5">
-        <v>264.91885000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="16:23" x14ac:dyDescent="0.3">
+        <v>265.60469999999998</v>
+      </c>
+      <c r="Y33" s="12"/>
+    </row>
+    <row r="34" spans="16:25" x14ac:dyDescent="0.3">
       <c r="P34" s="11" t="s">
         <v>19</v>
       </c>
@@ -1367,13 +1369,14 @@
         <v>42.141710000000003</v>
       </c>
       <c r="V34" s="1">
-        <v>44.538919999999997</v>
+        <v>45.288699999999999</v>
       </c>
       <c r="W34" s="1">
-        <v>20.057162999999999</v>
-      </c>
-    </row>
-    <row r="35" spans="16:23" x14ac:dyDescent="0.3">
+        <v>19.935879</v>
+      </c>
+      <c r="Y34" s="12"/>
+    </row>
+    <row r="35" spans="16:25" x14ac:dyDescent="0.3">
       <c r="P35" s="11" t="s">
         <v>20</v>
       </c>
@@ -1390,29 +1393,153 @@
         <v>348.78550000000001</v>
       </c>
       <c r="V35" s="1">
-        <v>336.62371999999999</v>
+        <v>336.98630000000003</v>
       </c>
       <c r="W35" s="1">
-        <v>321.56155000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="16:23" x14ac:dyDescent="0.3">
-      <c r="Q37" t="s">
+        <v>322.4341</v>
+      </c>
+      <c r="Y35" s="12"/>
+    </row>
+    <row r="36" spans="16:25" x14ac:dyDescent="0.3">
+      <c r="P36" s="16"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="Y36" s="12"/>
+    </row>
+    <row r="37" spans="16:25" x14ac:dyDescent="0.3">
+      <c r="P37" s="16"/>
+      <c r="Q37" s="1">
+        <v>6</v>
+      </c>
+      <c r="R37" s="1">
+        <v>5</v>
+      </c>
+      <c r="S37" s="1">
+        <v>4</v>
+      </c>
+      <c r="T37" s="1">
+        <v>3</v>
+      </c>
+      <c r="V37" s="1">
+        <v>2</v>
+      </c>
+      <c r="W37" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y37" s="12"/>
+    </row>
+    <row r="38" spans="16:25" x14ac:dyDescent="0.3">
+      <c r="P38" s="16"/>
+      <c r="Q38" s="1">
+        <v>5</v>
+      </c>
+      <c r="R38" s="1">
+        <v>6</v>
+      </c>
+      <c r="S38" s="1">
+        <v>1</v>
+      </c>
+      <c r="T38" s="1">
+        <v>3</v>
+      </c>
+      <c r="V38" s="1">
+        <v>4</v>
+      </c>
+      <c r="W38" s="1">
+        <v>2</v>
+      </c>
+      <c r="Y38" s="12"/>
+    </row>
+    <row r="39" spans="16:25" x14ac:dyDescent="0.3">
+      <c r="P39" s="16"/>
+      <c r="Q39" s="1">
+        <v>6</v>
+      </c>
+      <c r="R39" s="1">
+        <v>4</v>
+      </c>
+      <c r="S39" s="1">
+        <v>5</v>
+      </c>
+      <c r="T39" s="1">
+        <v>3</v>
+      </c>
+      <c r="V39" s="1">
+        <v>2</v>
+      </c>
+      <c r="W39" s="1">
+        <v>1</v>
+      </c>
+      <c r="Y39" s="12"/>
+    </row>
+    <row r="40" spans="16:25" x14ac:dyDescent="0.3">
+      <c r="Q40">
+        <f t="shared" ref="Q40:V40" si="0">AVERAGE(Q37:Q39)</f>
+        <v>5.666666666666667</v>
+      </c>
+      <c r="R40">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="S40">
+        <f t="shared" si="0"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="T40">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="V40">
+        <f t="shared" si="0"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="W40">
+        <f>AVERAGE(W37:W39)</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="41" spans="16:25" x14ac:dyDescent="0.3">
+      <c r="Q41" s="1">
+        <v>6</v>
+      </c>
+      <c r="R41" s="1">
+        <v>5</v>
+      </c>
+      <c r="S41" s="1">
+        <v>4</v>
+      </c>
+      <c r="T41" s="1">
+        <v>3</v>
+      </c>
+      <c r="V41" s="1">
+        <v>2</v>
+      </c>
+      <c r="W41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="16:25" x14ac:dyDescent="0.3">
+      <c r="Q42" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="38" spans="16:23" x14ac:dyDescent="0.3">
-      <c r="Q38" t="s">
+    <row r="43" spans="16:25" x14ac:dyDescent="0.3">
+      <c r="Q43" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="16:23" x14ac:dyDescent="0.3">
-      <c r="Q39" t="s">
+    <row r="44" spans="16:25" x14ac:dyDescent="0.3">
+      <c r="Q44" t="s">
         <v>23</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="Q31:W31"/>
     <mergeCell ref="X16:AA16"/>
     <mergeCell ref="W15:X15"/>
     <mergeCell ref="P30:Q30"/>
@@ -1420,7 +1547,6 @@
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="J16:M16"/>
     <mergeCell ref="Q16:T16"/>
-    <mergeCell ref="Q31:W31"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
non weighted working perfectly
</commit_message>
<xml_diff>
--- a/2 PART MIXTURE/Tables.xlsx
+++ b/2 PART MIXTURE/Tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\RAND_pro\prog_calc\prog_calc2\2 PART MIXTURE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1AA6F1-A492-416C-BB0E-5E5E97BC0020}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{309B49F7-7EE1-4E20-B59F-F8AF24A8F64C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{03F6D715-826B-4640-9764-84D30B4B9310}"/>
   </bookViews>
@@ -247,10 +247,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -568,7 +568,7 @@
   <dimension ref="B5:AG44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J22" workbookViewId="0">
-      <selection activeCell="Y39" sqref="Y39"/>
+      <selection activeCell="S35" sqref="S35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -586,12 +586,12 @@
       </c>
     </row>
     <row r="6" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
     </row>
     <row r="7" spans="2:27" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
@@ -702,36 +702,36 @@
       <c r="P15" t="s">
         <v>10</v>
       </c>
-      <c r="W15" s="15" t="s">
+      <c r="W15" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="X15" s="15"/>
+      <c r="X15" s="16"/>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.3">
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="J16" s="15" t="s">
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="J16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="Q16" s="15" t="s">
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="Q16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="X16" s="15" t="s">
+      <c r="R16" s="16"/>
+      <c r="S16" s="16"/>
+      <c r="T16" s="16"/>
+      <c r="X16" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
-      <c r="AA16" s="15"/>
+      <c r="Y16" s="16"/>
+      <c r="Z16" s="16"/>
+      <c r="AA16" s="16"/>
     </row>
     <row r="17" spans="2:33" x14ac:dyDescent="0.3">
       <c r="C17" t="s">
@@ -1293,19 +1293,19 @@
       </c>
     </row>
     <row r="30" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
+      <c r="P30" s="16"/>
+      <c r="Q30" s="16"/>
     </row>
     <row r="31" spans="2:33" x14ac:dyDescent="0.3">
-      <c r="Q31" s="15" t="s">
+      <c r="Q31" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="R31" s="15"/>
-      <c r="S31" s="15"/>
-      <c r="T31" s="15"/>
-      <c r="U31" s="15"/>
-      <c r="V31" s="15"/>
-      <c r="W31" s="15"/>
+      <c r="R31" s="16"/>
+      <c r="S31" s="16"/>
+      <c r="T31" s="16"/>
+      <c r="U31" s="16"/>
+      <c r="V31" s="16"/>
+      <c r="W31" s="16"/>
     </row>
     <row r="32" spans="2:33" x14ac:dyDescent="0.3">
       <c r="P32" s="9"/>
@@ -1345,10 +1345,10 @@
         <v>291.1773</v>
       </c>
       <c r="V33" s="5">
-        <v>282.1859</v>
+        <v>282.18518</v>
       </c>
       <c r="W33" s="5">
-        <v>265.60469999999998</v>
+        <v>265.04007000000001</v>
       </c>
       <c r="Y33" s="12"/>
     </row>
@@ -1369,10 +1369,10 @@
         <v>42.141710000000003</v>
       </c>
       <c r="V34" s="1">
-        <v>45.288699999999999</v>
+        <v>45.293582999999998</v>
       </c>
       <c r="W34" s="1">
-        <v>19.935879</v>
+        <v>22.628164000000002</v>
       </c>
       <c r="Y34" s="12"/>
     </row>
@@ -1393,15 +1393,15 @@
         <v>348.78550000000001</v>
       </c>
       <c r="V35" s="1">
-        <v>336.98630000000003</v>
+        <v>336.98419999999999</v>
       </c>
       <c r="W35" s="1">
-        <v>322.4341</v>
+        <v>321.11603000000002</v>
       </c>
       <c r="Y35" s="12"/>
     </row>
     <row r="36" spans="16:25" x14ac:dyDescent="0.3">
-      <c r="P36" s="16"/>
+      <c r="P36" s="15"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
@@ -1411,7 +1411,7 @@
       <c r="Y36" s="12"/>
     </row>
     <row r="37" spans="16:25" x14ac:dyDescent="0.3">
-      <c r="P37" s="16"/>
+      <c r="P37" s="15"/>
       <c r="Q37" s="1">
         <v>6</v>
       </c>
@@ -1433,7 +1433,7 @@
       <c r="Y37" s="12"/>
     </row>
     <row r="38" spans="16:25" x14ac:dyDescent="0.3">
-      <c r="P38" s="16"/>
+      <c r="P38" s="15"/>
       <c r="Q38" s="1">
         <v>5</v>
       </c>
@@ -1455,7 +1455,7 @@
       <c r="Y38" s="12"/>
     </row>
     <row r="39" spans="16:25" x14ac:dyDescent="0.3">
-      <c r="P39" s="16"/>
+      <c r="P39" s="15"/>
       <c r="Q39" s="1">
         <v>6</v>
       </c>

</xml_diff>